<commit_message>
included shading over 30°C in behavior table again
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Behavior.xlsx
+++ b/data/input_operation/OperationScenario_Component_Behavior.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7864E028-3537-4DFA-88F6-C5883D87BD0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B43D50-7A7E-455A-8C23-347FF4440A87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Beh" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -920,7 +920,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
behavior results inserted into operation model
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Behavior.xlsx
+++ b/data/input_operation/OperationScenario_Component_Behavior.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC77AFA3-418F-48CF-9D9C-2D08B6E6206E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A22BFFF-5E27-AC4C-A8E2-463F71262136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
+    <workbookView xWindow="-3480" yWindow="-20080" windowWidth="25340" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Beh" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>ID_Behavior</t>
   </si>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -564,48 +564,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -621,7 +621,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -916,14 +916,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -976,7 +988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -990,10 +1002,10 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>0.5</v>
@@ -1008,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>500000</v>
+        <v>490700</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -1017,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>1000000</v>
+        <v>1298746.816666668</v>
       </c>
       <c r="O2" t="s">
         <v>18</v>
@@ -1026,6 +1038,112 @@
         <v>1</v>
       </c>
       <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>490700</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1368629.9833333339</v>
+      </c>
+      <c r="O3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>490700</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>1423140.6500000004</v>
+      </c>
+      <c r="O4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated 'OperationScenario_BehaviorProfile.xlsx', 'OperationScenario_Component_Behavior.xlsx' with most recent output from FLEX-Behavior.
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Behavior.xlsx
+++ b/data/input_operation/OperationScenario_Component_Behavior.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevanskorna/PycharmProjects/FLEX/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22352C2F-8E7D-BE42-BCC6-CC7F36B08853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FC7848-2AD1-534E-9772-C27B30BE48B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1300" yWindow="-19800" windowWidth="25340" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10840" yWindow="-19540" windowWidth="25340" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Beh" sheetId="1" r:id="rId1"/>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>490700</v>
+        <v>448000</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>1298746.816666668</v>
+        <v>1230954.866666666</v>
       </c>
       <c r="O2" t="s">
         <v>18</v>
@@ -1095,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="K3">
-        <v>490700</v>
+        <v>448000</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
@@ -1104,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="N3">
-        <v>1368629.9833333339</v>
+        <v>1298178.2</v>
       </c>
       <c r="O3" t="s">
         <v>18</v>
@@ -1148,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="K4">
-        <v>490700</v>
+        <v>448000</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
@@ -1157,7 +1157,7 @@
         <v>3</v>
       </c>
       <c r="N4">
-        <v>1423140.6500000004</v>
+        <v>1357429.8666666674</v>
       </c>
       <c r="O4" t="s">
         <v>18</v>
@@ -1201,8 +1201,8 @@
         <v>4</v>
       </c>
       <c r="K5">
-        <f>1090600/2</f>
-        <v>545300</v>
+        <f>896000/2</f>
+        <v>448000</v>
       </c>
       <c r="L5" t="s">
         <v>18</v>
@@ -1211,8 +1211,8 @@
         <v>4</v>
       </c>
       <c r="N5">
-        <f>2403236.95/2</f>
-        <v>1201618.4750000001</v>
+        <f>1850130.56666667/2</f>
+        <v>925065.28333333496</v>
       </c>
       <c r="O5" t="s">
         <v>18</v>
@@ -1256,8 +1256,8 @@
         <v>5</v>
       </c>
       <c r="K6">
-        <f>1090600/2</f>
-        <v>545300</v>
+        <f t="shared" ref="K6:K7" si="0">896000/2</f>
+        <v>448000</v>
       </c>
       <c r="L6" t="s">
         <v>18</v>
@@ -1266,8 +1266,8 @@
         <v>5</v>
       </c>
       <c r="N6">
-        <f>2539809.95/2</f>
-        <v>1269904.9750000001</v>
+        <f>1966341.89999999/2</f>
+        <v>983170.94999999495</v>
       </c>
       <c r="O6" t="s">
         <v>18</v>
@@ -1311,8 +1311,8 @@
         <v>6</v>
       </c>
       <c r="K7">
-        <f>1090600/2</f>
-        <v>545300</v>
+        <f t="shared" si="0"/>
+        <v>448000</v>
       </c>
       <c r="L7" t="s">
         <v>18</v>
@@ -1321,8 +1321,8 @@
         <v>6</v>
       </c>
       <c r="N7">
-        <f>2648781.78333334/2</f>
-        <v>1324390.8916666701</v>
+        <f>2096722.23333334/2</f>
+        <v>1048361.11666667</v>
       </c>
       <c r="O7" t="s">
         <v>18</v>
@@ -1366,8 +1366,8 @@
         <v>7</v>
       </c>
       <c r="K8" s="1">
-        <f>1871800/4</f>
-        <v>467950</v>
+        <f>1822800/4</f>
+        <v>455700</v>
       </c>
       <c r="L8" t="s">
         <v>18</v>
@@ -1376,8 +1376,8 @@
         <v>7</v>
       </c>
       <c r="N8">
-        <f>3114707.48333332/4</f>
-        <v>778676.87083332997</v>
+        <f>3078779.26666667/4</f>
+        <v>769694.81666666747</v>
       </c>
       <c r="O8" t="s">
         <v>18</v>
@@ -1421,8 +1421,8 @@
         <v>8</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" ref="K9:K10" si="0">1871800/4</f>
-        <v>467950</v>
+        <f t="shared" ref="K9:K10" si="1">1822800/4</f>
+        <v>455700</v>
       </c>
       <c r="L9" t="s">
         <v>18</v>
@@ -1431,8 +1431,8 @@
         <v>8</v>
       </c>
       <c r="N9">
-        <f>3324475.48333331/4</f>
-        <v>831118.87083332753</v>
+        <f>3286375.93333333/4</f>
+        <v>821593.98333333246</v>
       </c>
       <c r="O9" t="s">
         <v>18</v>
@@ -1476,8 +1476,8 @@
         <v>9</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="0"/>
-        <v>467950</v>
+        <f t="shared" si="1"/>
+        <v>455700</v>
       </c>
       <c r="L10" t="s">
         <v>18</v>
@@ -1486,8 +1486,8 @@
         <v>9</v>
       </c>
       <c r="N10">
-        <f>3549490.98333333/4</f>
-        <v>887372.74583333253</v>
+        <f>3487821.1/4</f>
+        <v>871955.27500000002</v>
       </c>
       <c r="O10" t="s">
         <v>18</v>

</xml_diff>